<commit_message>
用Netty 自己 实现 dubbo RPC
</commit_message>
<xml_diff>
--- a/netty-demo/document/design/示意图 .xlsx
+++ b/netty-demo/document/design/示意图 .xlsx
@@ -1,48 +1,383 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505" activeTab="1"/>
+    <workbookView windowWidth="18525" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -50,9 +385,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -61,10 +638,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -75,7 +699,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
@@ -89,15 +713,15 @@
       <xdr:row>96</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="60" name="圆角矩形 59"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6143626" y="15382876"/>
-          <a:ext cx="2714624" cy="1076324"/>
+          <a:off x="6143625" y="15382875"/>
+          <a:ext cx="2714625" cy="1076325"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -132,6 +756,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>输出流对象</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -150,14 +775,14 @@
       <xdr:row>96</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="64" name="矩形 63"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6991349" y="15763875"/>
+          <a:off x="6990715" y="15763875"/>
           <a:ext cx="1800225" cy="695325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -214,7 +839,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -222,7 +847,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2371725" y="3343275"/>
-          <a:ext cx="6533334" cy="3400000"/>
+          <a:ext cx="6532880" cy="3399790"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -252,7 +877,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -260,7 +885,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4343400" y="7124700"/>
-          <a:ext cx="2095238" cy="1752381"/>
+          <a:ext cx="2094865" cy="1751965"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -277,7 +902,7 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="768095" cy="275717"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="TextBox 3"/>
         <xdr:cNvSpPr txBox="1"/>
@@ -285,7 +910,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2857500" y="9753600"/>
-          <a:ext cx="768095" cy="275717"/>
+          <a:ext cx="767715" cy="275590"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -320,6 +945,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>模式 </a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -338,7 +964,7 @@
       <xdr:row>63</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="圆角矩形 4"/>
         <xdr:cNvSpPr/>
@@ -396,7 +1022,7 @@
       <xdr:row>78</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="矩形 5"/>
         <xdr:cNvSpPr/>
@@ -435,6 +1061,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>Client(Socket)</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -465,7 +1092,7 @@
       <xdr:row>79</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="7" name="矩形 6"/>
         <xdr:cNvSpPr/>
@@ -523,7 +1150,7 @@
       <xdr:row>79</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="矩形 7"/>
         <xdr:cNvSpPr/>
@@ -581,7 +1208,7 @@
       <xdr:row>67</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="椭圆 8"/>
         <xdr:cNvSpPr/>
@@ -637,7 +1264,7 @@
       <xdr:row>68</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="椭圆 9"/>
         <xdr:cNvSpPr/>
@@ -693,7 +1320,7 @@
       <xdr:row>68</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="11" name="椭圆 10"/>
         <xdr:cNvSpPr/>
@@ -749,7 +1376,7 @@
       <xdr:row>71</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="12" name="矩形 11"/>
         <xdr:cNvSpPr/>
@@ -805,7 +1432,7 @@
       <xdr:row>71</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="13" name="矩形 12"/>
         <xdr:cNvSpPr/>
@@ -857,7 +1484,7 @@
       <xdr:row>71</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="14" name="矩形 13"/>
         <xdr:cNvSpPr/>
@@ -917,7 +1544,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -925,7 +1552,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2505075" y="12030075"/>
-          <a:ext cx="890093" cy="298730"/>
+          <a:ext cx="889635" cy="298450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -955,7 +1582,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -963,7 +1590,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4105275" y="12020550"/>
-          <a:ext cx="890093" cy="298730"/>
+          <a:ext cx="889635" cy="298450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -985,7 +1612,7 @@
       <xdr:row>65</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="18" name="直接箭头连接符 17"/>
         <xdr:cNvCxnSpPr/>
@@ -1032,7 +1659,7 @@
       <xdr:row>65</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="20" name="直接箭头连接符 19"/>
         <xdr:cNvCxnSpPr>
@@ -1042,7 +1669,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3081338" y="10925175"/>
+          <a:off x="3081020" y="10925175"/>
           <a:ext cx="66675" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1082,7 +1709,7 @@
       <xdr:row>65</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="22" name="直接箭头连接符 21"/>
         <xdr:cNvCxnSpPr>
@@ -1092,7 +1719,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3914775" y="10953750"/>
-          <a:ext cx="709613" cy="323850"/>
+          <a:ext cx="709295" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1131,7 +1758,7 @@
       <xdr:row>69</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="24" name="直接连接符 23"/>
         <xdr:cNvCxnSpPr>
@@ -1142,7 +1769,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1">
           <a:off x="1581150" y="11639550"/>
-          <a:ext cx="14288" cy="333375"/>
+          <a:ext cx="13970" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1178,7 +1805,7 @@
       <xdr:row>76</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="26" name="直接连接符 25"/>
         <xdr:cNvCxnSpPr>
@@ -1225,7 +1852,7 @@
       <xdr:row>70</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="28" name="直接连接符 27"/>
         <xdr:cNvCxnSpPr>
@@ -1235,7 +1862,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1">
           <a:off x="3067050" y="11677650"/>
-          <a:ext cx="14288" cy="381000"/>
+          <a:ext cx="13970" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1271,7 +1898,7 @@
       <xdr:row>76</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="30" name="直接连接符 29"/>
         <xdr:cNvCxnSpPr>
@@ -1281,8 +1908,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3033713" y="12325350"/>
-          <a:ext cx="4762" cy="809625"/>
+          <a:off x="3033395" y="12325350"/>
+          <a:ext cx="5080" cy="809625"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1318,7 +1945,7 @@
       <xdr:row>76</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="32" name="直接连接符 31"/>
         <xdr:cNvCxnSpPr>
@@ -1328,8 +1955,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4586288" y="12315825"/>
-          <a:ext cx="52387" cy="828675"/>
+          <a:off x="4585970" y="12315825"/>
+          <a:ext cx="52705" cy="828675"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1365,7 +1992,7 @@
       <xdr:row>70</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="34" name="直接连接符 33"/>
         <xdr:cNvCxnSpPr>
@@ -1374,8 +2001,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4624388" y="11696700"/>
-          <a:ext cx="33337" cy="400050"/>
+          <a:off x="4624070" y="11696700"/>
+          <a:ext cx="33655" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1406,7 +2033,7 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="782394" cy="275717"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="35" name="TextBox 34"/>
         <xdr:cNvSpPr txBox="1"/>
@@ -1414,7 +2041,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7829550" y="9886950"/>
-          <a:ext cx="782394" cy="275717"/>
+          <a:ext cx="782320" cy="275590"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1449,6 +2076,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>模式 </a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1467,7 +2095,7 @@
       <xdr:row>61</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="36" name="圆角矩形 35"/>
         <xdr:cNvSpPr/>
@@ -1506,6 +2134,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>Server</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -1552,7 +2181,7 @@
       <xdr:row>83</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="37" name="矩形 36"/>
         <xdr:cNvSpPr/>
@@ -1591,6 +2220,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>Client(Socket)</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -1598,6 +2228,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>程序</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1616,7 +2247,7 @@
       <xdr:row>79</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="38" name="矩形 37"/>
         <xdr:cNvSpPr/>
@@ -1674,7 +2305,7 @@
       <xdr:row>79</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="39" name="矩形 38"/>
         <xdr:cNvSpPr/>
@@ -1732,7 +2363,7 @@
       <xdr:row>65</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="42" name="椭圆 41"/>
         <xdr:cNvSpPr/>
@@ -1788,7 +2419,7 @@
       <xdr:row>74</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="44" name="矩形 43"/>
         <xdr:cNvSpPr/>
@@ -1840,7 +2471,7 @@
       <xdr:row>74</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="45" name="矩形 44"/>
         <xdr:cNvSpPr/>
@@ -1900,7 +2531,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1908,7 +2539,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7829550" y="12477750"/>
-          <a:ext cx="890093" cy="298730"/>
+          <a:ext cx="889635" cy="298450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1938,7 +2569,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1946,7 +2577,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9401175" y="12506325"/>
-          <a:ext cx="890093" cy="298730"/>
+          <a:ext cx="889635" cy="298450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1968,7 +2599,7 @@
       <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="51" name="直接连接符 50"/>
         <xdr:cNvCxnSpPr>
@@ -2015,7 +2646,7 @@
       <xdr:row>67</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="53" name="直接连接符 52"/>
         <xdr:cNvCxnSpPr>
@@ -2025,7 +2656,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1">
           <a:off x="8296275" y="11210925"/>
-          <a:ext cx="33338" cy="285750"/>
+          <a:ext cx="33020" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2061,7 +2692,7 @@
       <xdr:row>77</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="54" name="直接连接符 53"/>
         <xdr:cNvCxnSpPr>
@@ -2072,7 +2703,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8305800" y="12753975"/>
-          <a:ext cx="23813" cy="485775"/>
+          <a:ext cx="23495" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2108,7 +2739,7 @@
       <xdr:row>77</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="55" name="直接连接符 54"/>
         <xdr:cNvCxnSpPr>
@@ -2118,8 +2749,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9882188" y="12753975"/>
-          <a:ext cx="61912" cy="495300"/>
+          <a:off x="9881870" y="12753975"/>
+          <a:ext cx="62230" cy="495300"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2155,7 +2786,7 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="63" name="直接连接符 62"/>
         <xdr:cNvCxnSpPr>
@@ -2165,7 +2796,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8329613" y="10515600"/>
+          <a:off x="8329295" y="10515600"/>
           <a:ext cx="2390775" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2202,7 +2833,7 @@
       <xdr:row>68</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="65" name="圆角矩形 64"/>
         <xdr:cNvSpPr/>
@@ -2270,7 +2901,7 @@
       <xdr:row>72</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="68" name="直接连接符 67"/>
         <xdr:cNvCxnSpPr>
@@ -2280,8 +2911,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8274597" y="11744325"/>
-          <a:ext cx="88353" cy="733425"/>
+          <a:off x="8274050" y="11744325"/>
+          <a:ext cx="88900" cy="733425"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2317,7 +2948,7 @@
       <xdr:row>72</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="70" name="直接连接符 69"/>
         <xdr:cNvCxnSpPr>
@@ -2363,7 +2994,7 @@
       <xdr:row>80</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="73" name="矩形 72"/>
         <xdr:cNvSpPr/>
@@ -2421,7 +3052,7 @@
       <xdr:row>80</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="74" name="矩形 73"/>
         <xdr:cNvSpPr/>
@@ -2479,7 +3110,7 @@
       <xdr:row>80</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="75" name="矩形 74"/>
         <xdr:cNvSpPr/>
@@ -2537,7 +3168,7 @@
       <xdr:row>67</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="76" name="椭圆 75"/>
         <xdr:cNvSpPr/>
@@ -2593,7 +3224,7 @@
       <xdr:row>74</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="77" name="矩形 76"/>
         <xdr:cNvSpPr/>
@@ -2649,7 +3280,7 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="78" name="矩形 77"/>
         <xdr:cNvSpPr/>
@@ -2701,7 +3332,7 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="79" name="矩形 78"/>
         <xdr:cNvSpPr/>
@@ -2761,7 +3392,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2769,7 +3400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12334875" y="12620625"/>
-          <a:ext cx="890093" cy="298730"/>
+          <a:ext cx="889635" cy="298450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2799,7 +3430,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2807,7 +3438,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13906500" y="12649200"/>
-          <a:ext cx="890093" cy="298730"/>
+          <a:ext cx="889635" cy="298450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2829,7 +3460,7 @@
       <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="82" name="直接连接符 81"/>
         <xdr:cNvCxnSpPr>
@@ -2875,7 +3506,7 @@
       <xdr:row>77</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="83" name="直接连接符 82"/>
         <xdr:cNvCxnSpPr>
@@ -2885,8 +3516,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="11339513" y="12811125"/>
-          <a:ext cx="14287" cy="485775"/>
+          <a:off x="11339195" y="12811125"/>
+          <a:ext cx="14605" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2922,7 +3553,7 @@
       <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="84" name="直接连接符 83"/>
         <xdr:cNvCxnSpPr>
@@ -2932,7 +3563,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1">
           <a:off x="12801600" y="11544300"/>
-          <a:ext cx="33338" cy="285750"/>
+          <a:ext cx="33020" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2968,7 +3599,7 @@
       <xdr:row>78</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="85" name="直接连接符 84"/>
         <xdr:cNvCxnSpPr>
@@ -2979,7 +3610,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12811125" y="12896850"/>
-          <a:ext cx="23813" cy="485775"/>
+          <a:ext cx="23495" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3015,7 +3646,7 @@
       <xdr:row>78</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="86" name="直接连接符 85"/>
         <xdr:cNvCxnSpPr>
@@ -3025,8 +3656,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="14387513" y="12896850"/>
-          <a:ext cx="61912" cy="495300"/>
+          <a:off x="14387195" y="12896850"/>
+          <a:ext cx="62230" cy="495300"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3062,7 +3693,7 @@
       <xdr:row>70</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="87" name="圆角矩形 86"/>
         <xdr:cNvSpPr/>
@@ -3130,7 +3761,7 @@
       <xdr:row>73</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="88" name="直接连接符 87"/>
         <xdr:cNvCxnSpPr>
@@ -3140,7 +3771,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="12753975" y="12153900"/>
-          <a:ext cx="25947" cy="466725"/>
+          <a:ext cx="25400" cy="466725"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3176,7 +3807,7 @@
       <xdr:row>73</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="89" name="直接连接符 88"/>
         <xdr:cNvCxnSpPr>
@@ -3222,7 +3853,7 @@
       <xdr:row>64</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="92" name="直接连接符 91"/>
         <xdr:cNvCxnSpPr>
@@ -3232,7 +3863,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11068050" y="10534650"/>
-          <a:ext cx="1766888" cy="590550"/>
+          <a:ext cx="1766570" cy="590550"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3268,14 +3899,14 @@
       <xdr:row>74</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="102" name="矩形 101"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5905501" y="12268199"/>
+          <a:off x="5905500" y="12267565"/>
           <a:ext cx="609600" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3324,7 +3955,7 @@
       <xdr:row>74</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="103" name="矩形 102"/>
         <xdr:cNvSpPr/>
@@ -3332,7 +3963,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6600825" y="11830050"/>
-          <a:ext cx="1066799" cy="1000125"/>
+          <a:ext cx="1066165" cy="1000125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3365,6 +3996,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>channel</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -3419,14 +4051,14 @@
       <xdr:row>78</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="107" name="矩形 106"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6496051" y="12982575"/>
+          <a:off x="6496050" y="12982575"/>
           <a:ext cx="609600" cy="466725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3475,7 +4107,7 @@
       <xdr:row>75</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="108" name="上下箭头 107"/>
         <xdr:cNvSpPr/>
@@ -3529,7 +4161,7 @@
       <xdr:row>81</xdr:row>
       <xdr:rowOff>128588</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="110" name="曲线连接符 109"/>
         <xdr:cNvCxnSpPr>
@@ -3540,7 +4172,7 @@
       <xdr:spPr>
         <a:xfrm rot="10800000" flipH="1">
           <a:off x="6315075" y="13449300"/>
-          <a:ext cx="485776" cy="566738"/>
+          <a:ext cx="485775" cy="566420"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector4">
           <a:avLst>
@@ -3582,7 +4214,7 @@
       <xdr:row>81</xdr:row>
       <xdr:rowOff>128588</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="33" name="肘形连接符 32"/>
         <xdr:cNvCxnSpPr>
@@ -3592,7 +4224,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipH="1">
-          <a:off x="6315074" y="10034588"/>
+          <a:off x="6314440" y="10034270"/>
           <a:ext cx="3095625" cy="3981450"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
@@ -3634,7 +4266,7 @@
       <xdr:row>95</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="59" name="流程图: 多文档 58"/>
         <xdr:cNvSpPr/>
@@ -3692,7 +4324,7 @@
       <xdr:row>93</xdr:row>
       <xdr:rowOff>166688</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="62" name="直接箭头连接符 61"/>
         <xdr:cNvCxnSpPr>
@@ -3702,8 +4334,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8791574" y="16006763"/>
-          <a:ext cx="762001" cy="104775"/>
+          <a:off x="8790940" y="16006445"/>
+          <a:ext cx="762635" cy="104775"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3742,7 +4374,7 @@
       <xdr:row>96</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="67" name="矩形 66"/>
         <xdr:cNvSpPr/>
@@ -3781,6 +4413,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>ByteBuffer</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -3801,7 +4434,6 @@
             <a:buSzTx/>
             <a:buFontTx/>
             <a:buNone/>
-            <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
           <a:r>
@@ -3853,7 +4485,7 @@
       <xdr:row>88</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="69" name="TextBox 68"/>
         <xdr:cNvSpPr txBox="1"/>
@@ -3903,6 +4535,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>尚硅谷</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3921,7 +4554,7 @@
       <xdr:row>91</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="90" name="直接箭头连接符 89"/>
         <xdr:cNvCxnSpPr/>
@@ -3968,7 +4601,7 @@
       <xdr:row>93</xdr:row>
       <xdr:rowOff>166688</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="93" name="直接箭头连接符 92"/>
         <xdr:cNvCxnSpPr>
@@ -3978,7 +4611,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5800725" y="15906750"/>
-          <a:ext cx="1190624" cy="204788"/>
+          <a:ext cx="1189990" cy="204470"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4017,15 +4650,15 @@
       <xdr:row>96</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="111" name="圆角矩形 110"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11001376" y="15420976"/>
-          <a:ext cx="2714624" cy="1076324"/>
+          <a:off x="11001375" y="15420975"/>
+          <a:ext cx="2714625" cy="1076325"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4060,6 +4693,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>输入流对象</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4078,14 +4712,14 @@
       <xdr:row>96</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="112" name="矩形 111"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11849099" y="15801975"/>
+          <a:off x="11848465" y="15801975"/>
           <a:ext cx="1800225" cy="695325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4134,7 +4768,7 @@
       <xdr:row>94</xdr:row>
       <xdr:rowOff>33338</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="114" name="直接箭头连接符 113"/>
         <xdr:cNvCxnSpPr>
@@ -4144,7 +4778,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10306050" y="16030575"/>
-          <a:ext cx="1543049" cy="119063"/>
+          <a:ext cx="1542415" cy="118745"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4183,7 +4817,7 @@
       <xdr:row>95</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="115" name="矩形 114"/>
         <xdr:cNvSpPr/>
@@ -4222,6 +4856,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>ByteBuffer</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -4260,7 +4895,7 @@
       <xdr:row>94</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="117" name="直接箭头连接符 116"/>
         <xdr:cNvCxnSpPr>
@@ -4269,8 +4904,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="13477875" y="16006763"/>
-          <a:ext cx="704850" cy="233362"/>
+          <a:off x="13477875" y="16006445"/>
+          <a:ext cx="704850" cy="233680"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4309,7 +4944,7 @@
       <xdr:row>90</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="119" name="直接箭头连接符 118"/>
         <xdr:cNvCxnSpPr/>
@@ -4356,7 +4991,7 @@
       <xdr:row>88</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="120" name="TextBox 119"/>
         <xdr:cNvSpPr txBox="1"/>
@@ -4402,6 +5037,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>显示</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4420,14 +5056,14 @@
       <xdr:row>112</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="121" name="流程图: 多文档 120"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4686300" y="18659474"/>
+          <a:off x="4686300" y="18658840"/>
           <a:ext cx="895350" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartMultidocument">
@@ -4459,6 +5095,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>1.txt</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -4485,15 +5122,15 @@
       <xdr:row>113</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="122" name="圆角矩形 121"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6134101" y="18411825"/>
-          <a:ext cx="2714624" cy="1076324"/>
+          <a:off x="6134100" y="18411825"/>
+          <a:ext cx="2714625" cy="1075690"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4528,6 +5165,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>输入流对象</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4546,14 +5184,14 @@
       <xdr:row>113</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="123" name="矩形 122"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6981824" y="18792824"/>
+          <a:off x="6981190" y="18792190"/>
           <a:ext cx="1800225" cy="695325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4602,7 +5240,7 @@
       <xdr:row>111</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="124" name="直接箭头连接符 123"/>
         <xdr:cNvCxnSpPr>
@@ -4611,8 +5249,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5438775" y="19021424"/>
-          <a:ext cx="1543049" cy="119063"/>
+          <a:off x="5438775" y="19020790"/>
+          <a:ext cx="1542415" cy="119380"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4651,14 +5289,14 @@
       <xdr:row>113</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="125" name="矩形 124"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9315450" y="18564224"/>
+          <a:off x="9315450" y="18563590"/>
           <a:ext cx="1057275" cy="866775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4690,6 +5328,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>ByteBuffer</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -4728,7 +5367,7 @@
       <xdr:row>112</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="126" name="直接箭头连接符 125"/>
         <xdr:cNvCxnSpPr>
@@ -4737,8 +5376,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8610600" y="18997612"/>
-          <a:ext cx="704850" cy="233362"/>
+          <a:off x="8610600" y="18997295"/>
+          <a:ext cx="704850" cy="233045"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4777,14 +5416,14 @@
       <xdr:row>112</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="127" name="流程图: 多文档 126"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13935075" y="18640424"/>
+          <a:off x="13935075" y="18639790"/>
           <a:ext cx="895350" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartMultidocument">
@@ -4816,6 +5455,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>2.txt</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -4842,15 +5482,15 @@
       <xdr:row>114</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="128" name="圆角矩形 127"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10915651" y="18497551"/>
-          <a:ext cx="2714624" cy="1076324"/>
+          <a:off x="10915650" y="18497550"/>
+          <a:ext cx="2714625" cy="1076325"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4885,6 +5525,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>输出流对象</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4903,14 +5544,14 @@
       <xdr:row>114</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="129" name="矩形 128"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11763374" y="18878550"/>
+          <a:off x="11762740" y="18878550"/>
           <a:ext cx="1800225" cy="695325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4959,7 +5600,7 @@
       <xdr:row>112</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="131" name="直接箭头连接符 130"/>
         <xdr:cNvCxnSpPr/>
@@ -5006,7 +5647,7 @@
       <xdr:row>113</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="133" name="直接箭头连接符 132"/>
         <xdr:cNvCxnSpPr>
@@ -5015,8 +5656,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="13249275" y="18978562"/>
-          <a:ext cx="685800" cy="404813"/>
+          <a:off x="13249275" y="18978245"/>
+          <a:ext cx="685800" cy="405130"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5063,7 +5704,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5075,10 +5716,10 @@
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="1657350" y="20364450"/>
-          <a:ext cx="6905625" cy="3816674"/>
+          <a:ext cx="6905625" cy="3816350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5141,7 +5782,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5153,10 +5794,10 @@
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8750300" y="24338187"/>
-          <a:ext cx="2600755" cy="1053537"/>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8724900" y="24640540"/>
+          <a:ext cx="2592070" cy="1066165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5219,7 +5860,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+        <a:blip r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5231,10 +5872,10 @@
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10634456" y="23426403"/>
-          <a:ext cx="2808312" cy="966796"/>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10634345" y="23425785"/>
+          <a:ext cx="2807970" cy="967105"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5297,7 +5938,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+        <a:blip r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5309,10 +5950,10 @@
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="12596490" y="24711371"/>
-          <a:ext cx="2520280" cy="819401"/>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12595860" y="24711025"/>
+          <a:ext cx="2520315" cy="819150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5375,7 +6016,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+        <a:blip r:embed="rId8">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5387,10 +6028,10 @@
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8948920" y="20221575"/>
-          <a:ext cx="3423328" cy="1560457"/>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8948420" y="20221575"/>
+          <a:ext cx="3423285" cy="1560195"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5453,7 +6094,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+        <a:blip r:embed="rId9">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5465,9 +6106,9 @@
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8948920" y="21884280"/>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8948420" y="21884005"/>
           <a:ext cx="7134225" cy="895350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5523,15 +6164,15 @@
       <xdr:row>150</xdr:row>
       <xdr:rowOff>126999</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="17" name="TextBox 16"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2973917" y="24045332"/>
-          <a:ext cx="5408083" cy="1481667"/>
+          <a:off x="2965450" y="24343360"/>
+          <a:ext cx="5391150" cy="1500505"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5588,6 +6229,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>6667</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
@@ -5610,6 +6252,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>]</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
@@ -5674,15 +6317,15 @@
       <xdr:rowOff>52917</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1172116" cy="275717"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="19" name="TextBox 18"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4656667" y="27654250"/>
-          <a:ext cx="1172116" cy="275717"/>
+          <a:off x="4643755" y="27999055"/>
+          <a:ext cx="1172210" cy="275590"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5713,6 +6356,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>链式操作示意图</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5731,15 +6375,15 @@
       <xdr:row>177</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="21" name="矩形 20"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3291417" y="29389917"/>
-          <a:ext cx="1365250" cy="687916"/>
+          <a:off x="3282950" y="29756100"/>
+          <a:ext cx="1360805" cy="695960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5770,6 +6414,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>读取数据</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5788,15 +6433,15 @@
       <xdr:row>177</xdr:row>
       <xdr:rowOff>99483</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="104" name="矩形 103"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5613400" y="29383567"/>
-          <a:ext cx="1365250" cy="687916"/>
+          <a:off x="5596255" y="29749750"/>
+          <a:ext cx="1360805" cy="695960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5862,15 +6507,15 @@
       <xdr:row>177</xdr:row>
       <xdr:rowOff>93133</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="105" name="矩形 104"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7575550" y="29377217"/>
-          <a:ext cx="1365250" cy="687916"/>
+          <a:off x="7552055" y="29743400"/>
+          <a:ext cx="1363345" cy="695960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5924,15 +6569,15 @@
       <xdr:row>177</xdr:row>
       <xdr:rowOff>86783</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="106" name="矩形 105"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9421283" y="29370867"/>
-          <a:ext cx="1365250" cy="687916"/>
+          <a:off x="9393555" y="29737050"/>
+          <a:ext cx="1360805" cy="695960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5979,6 +6624,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>)</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -6001,15 +6647,15 @@
       <xdr:row>177</xdr:row>
       <xdr:rowOff>59266</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="109" name="矩形 108"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11499849" y="29343350"/>
-          <a:ext cx="1365250" cy="687916"/>
+          <a:off x="11465560" y="29709110"/>
+          <a:ext cx="1360805" cy="696595"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6063,7 +6709,7 @@
       <xdr:row>175</xdr:row>
       <xdr:rowOff>100542</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="25" name="肘形连接符 24"/>
         <xdr:cNvCxnSpPr>
@@ -6073,8 +6719,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4656667" y="29727525"/>
-          <a:ext cx="956733" cy="6350"/>
+          <a:off x="4643755" y="30097730"/>
+          <a:ext cx="952500" cy="6350"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -6113,7 +6759,7 @@
       <xdr:row>175</xdr:row>
       <xdr:rowOff>94192</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="29" name="肘形连接符 28"/>
         <xdr:cNvCxnSpPr>
@@ -6123,8 +6769,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6978650" y="29721175"/>
-          <a:ext cx="596900" cy="6350"/>
+          <a:off x="6957060" y="30091380"/>
+          <a:ext cx="594995" cy="6350"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -6163,15 +6809,15 @@
       <xdr:row>176</xdr:row>
       <xdr:rowOff>84666</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="40" name="肘形连接符 39"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8953500" y="29601583"/>
-          <a:ext cx="497417" cy="285750"/>
+          <a:off x="8925560" y="29969460"/>
+          <a:ext cx="497840" cy="290195"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -6210,7 +6856,7 @@
       <xdr:row>176</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="43" name="肘形连接符 42"/>
         <xdr:cNvCxnSpPr>
@@ -6219,8 +6865,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10795000" y="29687308"/>
-          <a:ext cx="704849" cy="210609"/>
+          <a:off x="10763250" y="30057725"/>
+          <a:ext cx="702310" cy="212725"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -6259,15 +6905,15 @@
       <xdr:row>185</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="48" name="圆角矩形 47"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5598583" y="30638750"/>
-          <a:ext cx="1397000" cy="719667"/>
+          <a:off x="5581650" y="31019750"/>
+          <a:ext cx="1392555" cy="730250"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6315,15 +6961,15 @@
       <xdr:row>185</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="116" name="圆角矩形 115"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7507816" y="30664150"/>
-          <a:ext cx="1397000" cy="719667"/>
+          <a:off x="7486015" y="31047055"/>
+          <a:ext cx="1393190" cy="728345"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6371,15 +7017,15 @@
       <xdr:row>185</xdr:row>
       <xdr:rowOff>61384</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="118" name="圆角矩形 117"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9385300" y="30668384"/>
-          <a:ext cx="1397000" cy="719667"/>
+          <a:off x="9357360" y="31051500"/>
+          <a:ext cx="1393190" cy="727710"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6427,15 +7073,15 @@
       <xdr:row>185</xdr:row>
       <xdr:rowOff>118534</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="130" name="圆角矩形 129"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11569700" y="30725534"/>
-          <a:ext cx="1397000" cy="719667"/>
+          <a:off x="11535410" y="31108650"/>
+          <a:ext cx="1393190" cy="727710"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6483,7 +7129,7 @@
       <xdr:row>180</xdr:row>
       <xdr:rowOff>148168</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="50" name="曲线连接符 49"/>
         <xdr:cNvCxnSpPr>
@@ -6492,8 +7138,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="5854171" y="30186313"/>
-          <a:ext cx="556684" cy="327025"/>
+          <a:off x="5832475" y="30565090"/>
+          <a:ext cx="563245" cy="324485"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -6532,15 +7178,15 @@
       <xdr:row>181</xdr:row>
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="56" name="曲线连接符 55"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="7852834" y="30130750"/>
-          <a:ext cx="613833" cy="465666"/>
+          <a:off x="7823835" y="30510480"/>
+          <a:ext cx="622300" cy="463550"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -6579,15 +7225,15 @@
       <xdr:row>181</xdr:row>
       <xdr:rowOff>42334</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="58" name="曲线连接符 57"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="9667875" y="30114875"/>
-          <a:ext cx="613834" cy="539750"/>
+          <a:off x="9633585" y="30493335"/>
+          <a:ext cx="622300" cy="539750"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -6626,15 +7272,15 @@
       <xdr:row>181</xdr:row>
       <xdr:rowOff>74084</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="66" name="曲线连接符 65"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="11890375" y="30273625"/>
-          <a:ext cx="635000" cy="264584"/>
+          <a:off x="11849735" y="30652085"/>
+          <a:ext cx="643890" cy="264795"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -6673,7 +7319,7 @@
       <xdr:row>181</xdr:row>
       <xdr:rowOff>74085</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="91" name="曲线连接符 90"/>
         <xdr:cNvCxnSpPr>
@@ -6682,8 +7328,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="3590396" y="30339771"/>
-          <a:ext cx="645584" cy="121709"/>
+          <a:off x="3575050" y="30718125"/>
+          <a:ext cx="654050" cy="121920"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -6722,15 +7368,15 @@
       <xdr:row>189</xdr:row>
       <xdr:rowOff>42333</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="132" name="圆角矩形 131"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2935815" y="30738233"/>
-          <a:ext cx="2038351" cy="1308100"/>
+          <a:off x="2926715" y="31121350"/>
+          <a:ext cx="2032000" cy="1324610"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6759,6 +7405,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>handler</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -6798,6 +7445,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>实现异步</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6816,15 +7464,15 @@
       <xdr:row>200</xdr:row>
       <xdr:rowOff>116416</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="100" name="圆角矩形 99"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5461000" y="33009417"/>
-          <a:ext cx="1629833" cy="973666"/>
+          <a:off x="5445760" y="33420050"/>
+          <a:ext cx="1623695" cy="986155"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6874,15 +7522,15 @@
       <xdr:row>214</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="101" name="圆角矩形 100"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3958166" y="35411833"/>
-          <a:ext cx="1174750" cy="825500"/>
+          <a:off x="3947160" y="35854005"/>
+          <a:ext cx="1170305" cy="836295"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6936,15 +7584,15 @@
       <xdr:row>214</xdr:row>
       <xdr:rowOff>46567</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="134" name="圆角矩形 133"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6491816" y="35458400"/>
-          <a:ext cx="1174750" cy="825500"/>
+          <a:off x="6472555" y="35900360"/>
+          <a:ext cx="1170305" cy="836295"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6998,7 +7646,7 @@
       <xdr:row>209</xdr:row>
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="135" name="曲线连接符 134"/>
         <xdr:cNvCxnSpPr>
@@ -7007,8 +7655,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="4553479" y="34006895"/>
-          <a:ext cx="1397000" cy="1412876"/>
+          <a:off x="4528820" y="34441765"/>
+          <a:ext cx="1416050" cy="1408430"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector2">
           <a:avLst/>
@@ -7047,15 +7695,15 @@
       <xdr:row>200</xdr:row>
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="136" name="圆角矩形 135"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5588000" y="33506833"/>
-          <a:ext cx="624417" cy="381000"/>
+          <a:off x="5570855" y="33923605"/>
+          <a:ext cx="622300" cy="387350"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -7103,15 +7751,15 @@
       <xdr:row>209</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="138" name="曲线连接符 137"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="6201833" y="34321750"/>
-          <a:ext cx="1534584" cy="730250"/>
+          <a:off x="6171565" y="34755455"/>
+          <a:ext cx="1553845" cy="727710"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -7150,15 +7798,15 @@
       <xdr:row>200</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="139" name="圆角矩形 138"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6364817" y="33511067"/>
-          <a:ext cx="624417" cy="381000"/>
+          <a:off x="6345555" y="33928050"/>
+          <a:ext cx="622300" cy="387350"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -7206,15 +7854,15 @@
       <xdr:row>234</xdr:row>
       <xdr:rowOff>21167</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="23" name="TextBox 22"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1238250" y="37147500"/>
-          <a:ext cx="5111750" cy="2497667"/>
+          <a:off x="1235710" y="37611050"/>
+          <a:ext cx="5095240" cy="2529205"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7411,15 +8059,15 @@
       <xdr:row>234</xdr:row>
       <xdr:rowOff>10583</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="27" name="矩形 26"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7281332" y="37073416"/>
-          <a:ext cx="8339668" cy="2561167"/>
+          <a:off x="7259955" y="37534215"/>
+          <a:ext cx="8314055" cy="2595245"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7469,15 +8117,15 @@
       <xdr:row>230</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="31" name="圆角矩形 30"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5132917" y="38015333"/>
-          <a:ext cx="1449916" cy="994834"/>
+          <a:off x="5118100" y="38489255"/>
+          <a:ext cx="1445260" cy="1007745"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -7508,6 +8156,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>socket</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -7519,6 +8168,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>二进制字节码</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7537,7 +8187,7 @@
       <xdr:row>227</xdr:row>
       <xdr:rowOff>74083</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="49" name="肘形连接符 48"/>
         <xdr:cNvCxnSpPr>
@@ -7546,8 +8196,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6582833" y="38163500"/>
-          <a:ext cx="603250" cy="349250"/>
+          <a:off x="6563360" y="38639750"/>
+          <a:ext cx="601345" cy="353060"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -7586,15 +8236,15 @@
       <xdr:row>232</xdr:row>
       <xdr:rowOff>116417</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="52" name="圆角矩形 51"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7365999" y="37835417"/>
-          <a:ext cx="6858001" cy="1566333"/>
+          <a:off x="7344410" y="38307010"/>
+          <a:ext cx="6837045" cy="1585595"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -7623,6 +8273,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>ToIntegerDecoder</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -7645,15 +8296,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="57" name="矩形 56"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7598833" y="38491584"/>
-          <a:ext cx="3503084" cy="381000"/>
+          <a:off x="7575550" y="38971855"/>
+          <a:ext cx="3492500" cy="385445"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7694,15 +8345,15 @@
       <xdr:rowOff>127001</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="918778" cy="275717"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="61" name="TextBox 60"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7567083" y="38904334"/>
-          <a:ext cx="918778" cy="275717"/>
+          <a:off x="7543800" y="39389050"/>
+          <a:ext cx="918210" cy="275590"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7756,15 +8407,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>52917</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="71" name="矩形 70"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7641167" y="38565667"/>
-          <a:ext cx="370416" cy="264583"/>
+          <a:off x="7617460" y="39046150"/>
+          <a:ext cx="370840" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7812,15 +8463,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>4234</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="137" name="矩形 136"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8566150" y="38516984"/>
-          <a:ext cx="370416" cy="264583"/>
+          <a:off x="8540750" y="38997255"/>
+          <a:ext cx="370205" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7868,15 +8519,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>61384</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="140" name="矩形 139"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9448800" y="38574134"/>
-          <a:ext cx="370416" cy="264583"/>
+          <a:off x="9420860" y="39054405"/>
+          <a:ext cx="368300" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7924,15 +8575,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="141" name="矩形 140"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10606617" y="38588950"/>
-          <a:ext cx="370416" cy="264583"/>
+          <a:off x="10574655" y="39069010"/>
+          <a:ext cx="370205" cy="269240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7980,15 +8631,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>59267</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="142" name="矩形 141"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9795933" y="38572017"/>
-          <a:ext cx="370416" cy="264583"/>
+          <a:off x="9766300" y="39052500"/>
+          <a:ext cx="370205" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8036,15 +8687,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>74084</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="143" name="矩形 142"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10202334" y="38586834"/>
-          <a:ext cx="370416" cy="264583"/>
+          <a:off x="10172700" y="39067105"/>
+          <a:ext cx="368300" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8092,15 +8743,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>25401</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="144" name="矩形 143"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8142816" y="38538151"/>
-          <a:ext cx="370416" cy="264583"/>
+          <a:off x="8119110" y="39018210"/>
+          <a:ext cx="368300" cy="269240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8148,15 +8799,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>29632</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="145" name="矩形 144"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9014884" y="38542382"/>
-          <a:ext cx="370416" cy="264583"/>
+          <a:off x="8987155" y="39022655"/>
+          <a:ext cx="370205" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8204,15 +8855,15 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>84667</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="72" name="圆角矩形 71"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11207751" y="38258750"/>
-          <a:ext cx="825500" cy="603250"/>
+          <a:off x="11173460" y="38735000"/>
+          <a:ext cx="823595" cy="611505"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -8262,15 +8913,15 @@
       <xdr:row>231</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="113" name="圆角矩形 112"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12213168" y="38068250"/>
-          <a:ext cx="1079500" cy="1153583"/>
+          <a:off x="12176760" y="38541960"/>
+          <a:ext cx="1075690" cy="1168400"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -8301,6 +8952,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>list</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -8323,15 +8975,15 @@
       <xdr:row>228</xdr:row>
       <xdr:rowOff>74083</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="146" name="矩形 145"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12308417" y="38385750"/>
-          <a:ext cx="857250" cy="296333"/>
+          <a:off x="12272010" y="38863905"/>
+          <a:ext cx="853440" cy="300355"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8379,15 +9031,15 @@
       <xdr:row>234</xdr:row>
       <xdr:rowOff>74084</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="148" name="直接箭头连接符 147"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11080750" y="38859884"/>
-          <a:ext cx="45508" cy="838200"/>
+          <a:off x="11046460" y="39344600"/>
+          <a:ext cx="45720" cy="848360"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8426,15 +9078,15 @@
       <xdr:row>231</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="149" name="矩形 148"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12312650" y="38766750"/>
-          <a:ext cx="857250" cy="349250"/>
+          <a:off x="12276455" y="39249350"/>
+          <a:ext cx="852805" cy="355600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8482,7 +9134,7 @@
       <xdr:row>231</xdr:row>
       <xdr:rowOff>105832</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="151" name="肘形连接符 150"/>
         <xdr:cNvCxnSpPr>
@@ -8492,8 +9144,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="12006793" y="38475707"/>
-          <a:ext cx="359833" cy="1132417"/>
+          <a:off x="11968480" y="38964235"/>
+          <a:ext cx="363855" cy="1128395"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -8534,15 +9186,15 @@
       <xdr:row>232</xdr:row>
       <xdr:rowOff>137584</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="152" name="矩形 151"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14562667" y="37793083"/>
-          <a:ext cx="1037166" cy="1629834"/>
+          <a:off x="14518005" y="38265100"/>
+          <a:ext cx="1035050" cy="1648460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8573,6 +9225,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>ChannelInboundHandler</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -8607,7 +9260,7 @@
       <xdr:row>228</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="154" name="肘形连接符 153"/>
         <xdr:cNvCxnSpPr>
@@ -8616,8 +9269,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13197417" y="38555083"/>
-          <a:ext cx="1365250" cy="52917"/>
+          <a:off x="13157200" y="39035355"/>
+          <a:ext cx="1360805" cy="55245"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -8656,7 +9309,7 @@
       <xdr:row>224</xdr:row>
       <xdr:rowOff>84665</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="156" name="肘形连接符 155"/>
         <xdr:cNvCxnSpPr>
@@ -8665,8 +9318,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="5857875" y="37464999"/>
-          <a:ext cx="1434042" cy="550333"/>
+          <a:off x="5840730" y="37932360"/>
+          <a:ext cx="1430020" cy="556895"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -8705,15 +9358,15 @@
       <xdr:row>222</xdr:row>
       <xdr:rowOff>84667</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="157" name="圆角矩形 156"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8466667" y="37221583"/>
-          <a:ext cx="1788583" cy="455084"/>
+          <a:off x="8441055" y="37684710"/>
+          <a:ext cx="1784350" cy="461645"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -8751,7 +9404,6 @@
             <a:buSzTx/>
             <a:buFontTx/>
             <a:buNone/>
-            <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
           <a:r>
@@ -8791,15 +9443,15 @@
       <xdr:row>222</xdr:row>
       <xdr:rowOff>169332</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="158" name="圆角矩形 157"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10809817" y="37236399"/>
-          <a:ext cx="2091266" cy="524933"/>
+          <a:off x="10777855" y="37699315"/>
+          <a:ext cx="2084705" cy="531495"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -8847,7 +9499,7 @@
       <xdr:row>221</xdr:row>
       <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="160" name="直接箭头连接符 159"/>
         <xdr:cNvCxnSpPr>
@@ -8856,8 +9508,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="10255250" y="37449125"/>
-          <a:ext cx="497417" cy="79375"/>
+          <a:off x="10225405" y="37916485"/>
+          <a:ext cx="495300" cy="79375"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8896,7 +9548,7 @@
       <xdr:row>229</xdr:row>
       <xdr:rowOff>164042</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="168" name="肘形连接符 167"/>
         <xdr:cNvCxnSpPr>
@@ -8905,8 +9557,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="13169900" y="38851417"/>
-          <a:ext cx="1350433" cy="89958"/>
+          <a:off x="13129260" y="39335710"/>
+          <a:ext cx="1346200" cy="90170"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -8945,15 +9597,15 @@
       <xdr:row>254</xdr:row>
       <xdr:rowOff>52918</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="169" name="矩形 168"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1555749" y="41179750"/>
-          <a:ext cx="4021667" cy="1883835"/>
+          <a:off x="1551305" y="41694100"/>
+          <a:ext cx="4008755" cy="1906905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8982,6 +9634,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>Client</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -9012,15 +9665,15 @@
       <xdr:row>250</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="170" name="圆角矩形 169"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5683250" y="41931167"/>
-          <a:ext cx="2868083" cy="465666"/>
+          <a:off x="5666105" y="42453560"/>
+          <a:ext cx="2859405" cy="472440"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -9070,15 +9723,15 @@
       <xdr:row>254</xdr:row>
       <xdr:rowOff>35985</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="171" name="矩形 170"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8693149" y="40925750"/>
-          <a:ext cx="4021667" cy="2120902"/>
+          <a:off x="8667115" y="41435655"/>
+          <a:ext cx="4009390" cy="2148205"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9107,6 +9760,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>Server</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -9137,15 +9791,15 @@
       <xdr:row>253</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="172" name="矩形 171"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1746250" y="42079333"/>
-          <a:ext cx="952500" cy="857250"/>
+          <a:off x="1741805" y="42604055"/>
+          <a:ext cx="950595" cy="868045"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9195,15 +9849,15 @@
       <xdr:row>253</xdr:row>
       <xdr:rowOff>110067</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="174" name="矩形 173"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3052233" y="42475150"/>
-          <a:ext cx="1435099" cy="476250"/>
+          <a:off x="3043555" y="43004105"/>
+          <a:ext cx="1430655" cy="482600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9253,7 +9907,7 @@
       <xdr:row>252</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="175" name="曲线连接符 174"/>
         <xdr:cNvCxnSpPr>
@@ -9262,8 +9916,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2645833" y="42713275"/>
-          <a:ext cx="406400" cy="22225"/>
+          <a:off x="2639060" y="43246675"/>
+          <a:ext cx="404495" cy="22225"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -9302,7 +9956,7 @@
       <xdr:row>252</xdr:row>
       <xdr:rowOff>116417</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="177" name="曲线连接符 176"/>
         <xdr:cNvCxnSpPr>
@@ -9311,8 +9965,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4508500" y="42164000"/>
-          <a:ext cx="1174750" cy="624417"/>
+          <a:off x="4495800" y="42691050"/>
+          <a:ext cx="1170305" cy="630555"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -9351,15 +10005,15 @@
       <xdr:row>252</xdr:row>
       <xdr:rowOff>135467</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="179" name="矩形 178"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8930216" y="42331217"/>
-          <a:ext cx="1435099" cy="476250"/>
+          <a:off x="8904605" y="42858055"/>
+          <a:ext cx="1428750" cy="482600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9409,15 +10063,15 @@
       <xdr:row>252</xdr:row>
       <xdr:rowOff>148166</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="180" name="矩形 179"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10839450" y="41700449"/>
-          <a:ext cx="1435099" cy="1119717"/>
+          <a:off x="10807700" y="42220515"/>
+          <a:ext cx="1430655" cy="1132840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9467,7 +10121,7 @@
       <xdr:row>251</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="181" name="曲线连接符 180"/>
         <xdr:cNvCxnSpPr>
@@ -9476,8 +10130,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8445500" y="42312167"/>
-          <a:ext cx="484716" cy="257175"/>
+          <a:off x="8420100" y="42839005"/>
+          <a:ext cx="484505" cy="261620"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -9516,15 +10170,15 @@
       <xdr:row>252</xdr:row>
       <xdr:rowOff>21167</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="183" name="曲线连接符 182"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10297583" y="42322750"/>
-          <a:ext cx="518584" cy="370417"/>
+          <a:off x="10267950" y="42849800"/>
+          <a:ext cx="516255" cy="376555"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -9563,15 +10217,15 @@
       <xdr:row>248</xdr:row>
       <xdr:rowOff>33866</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="185" name="矩形 184"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8945033" y="41552283"/>
-          <a:ext cx="1435099" cy="476250"/>
+          <a:off x="8917305" y="42070655"/>
+          <a:ext cx="1430655" cy="482600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9621,7 +10275,7 @@
       <xdr:row>247</xdr:row>
       <xdr:rowOff>148167</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="186" name="曲线连接符 185"/>
         <xdr:cNvCxnSpPr>
@@ -9630,8 +10284,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="10380133" y="41790408"/>
-          <a:ext cx="467785" cy="183092"/>
+          <a:off x="10347960" y="42310685"/>
+          <a:ext cx="467995" cy="185420"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -9670,7 +10324,7 @@
       <xdr:row>248</xdr:row>
       <xdr:rowOff>21165</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="188" name="曲线连接符 187"/>
         <xdr:cNvCxnSpPr>
@@ -9679,8 +10333,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="8456083" y="41790407"/>
-          <a:ext cx="488950" cy="225425"/>
+          <a:off x="8430260" y="42310685"/>
+          <a:ext cx="487045" cy="229870"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -9719,15 +10373,15 @@
       <xdr:row>249</xdr:row>
       <xdr:rowOff>93133</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="190" name="矩形 189"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3067050" y="41780883"/>
-          <a:ext cx="1435099" cy="476250"/>
+          <a:off x="3058160" y="42301160"/>
+          <a:ext cx="1430655" cy="482600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9777,7 +10431,7 @@
       <xdr:row>248</xdr:row>
       <xdr:rowOff>24340</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="191" name="曲线连接符 190"/>
         <xdr:cNvCxnSpPr>
@@ -9786,8 +10440,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="4502149" y="41952332"/>
-          <a:ext cx="1202268" cy="66675"/>
+          <a:off x="4488815" y="42474515"/>
+          <a:ext cx="1198245" cy="69215"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -9826,15 +10480,15 @@
       <xdr:row>250</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="1026" name="曲线连接符 1025"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="2656418" y="42058167"/>
-          <a:ext cx="359833" cy="275166"/>
+          <a:off x="2649855" y="42583100"/>
+          <a:ext cx="357505" cy="279400"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -9881,7 +10535,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+        <a:blip r:embed="rId10">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -9893,10 +10547,10 @@
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6604000" y="45010917"/>
-          <a:ext cx="6281368" cy="5256560"/>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6584950" y="45571410"/>
+          <a:ext cx="6261735" cy="5322570"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9917,21 +10571,21 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
       <xdr:row>305</xdr:row>
-      <xdr:rowOff>148166</xdr:rowOff>
+      <xdr:rowOff>100330</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1772473" cy="275717"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="41" name="TextBox 40"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8699500" y="51794833"/>
-          <a:ext cx="1772473" cy="275717"/>
+          <a:off x="9645650" y="52392580"/>
+          <a:ext cx="1772285" cy="275590"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9997,7 +10651,7 @@
       <xdr:row>330</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="147" name="矩形 146"/>
         <xdr:cNvSpPr/>
@@ -10069,7 +10723,7 @@
       <xdr:row>331</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="150" name="圆角矩形 149"/>
         <xdr:cNvSpPr/>
@@ -10139,7 +10793,7 @@
       <xdr:row>313</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="153" name="圆角矩形 152"/>
         <xdr:cNvSpPr/>
@@ -10190,6 +10844,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
             <a:t> </a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -10216,7 +10871,7 @@
       <xdr:row>322</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="155" name="矩形 154"/>
         <xdr:cNvSpPr/>
@@ -10253,6 +10908,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>provider</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -10299,7 +10955,7 @@
       <xdr:row>328</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="159" name="矩形 158"/>
         <xdr:cNvSpPr/>
@@ -10338,6 +10994,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>netty </a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -10345,6 +11002,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>1. NettySever </a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -10371,7 +11029,7 @@
       <xdr:row>321</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="182" name="矩形 181"/>
         <xdr:cNvSpPr/>
@@ -10436,6 +11094,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
             <a:t>NettyClient</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -10466,7 +11125,7 @@
       <xdr:row>328</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="184" name="矩形 183"/>
         <xdr:cNvSpPr/>
@@ -10505,6 +11164,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>netty </a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -10512,6 +11172,7 @@
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
             <a:t>1. NettyClient</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -10528,28 +11189,30 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>318</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>318</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>318</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="1025" name="曲线连接符 1024"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8515350" y="54568725"/>
-          <a:ext cx="2971800" cy="95250"/>
+        <a:xfrm>
+          <a:off x="8820150" y="54663975"/>
+          <a:ext cx="2628900" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50024"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -10585,7 +11248,7 @@
       <xdr:row>313</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="1028" name="肘形连接符 1027"/>
         <xdr:cNvCxnSpPr>
@@ -10594,8 +11257,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="8172451" y="53359050"/>
-          <a:ext cx="1304929" cy="419100"/>
+          <a:off x="8172450" y="53359050"/>
+          <a:ext cx="1304925" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -10634,7 +11297,7 @@
       <xdr:row>313</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="1030" name="肘形连接符 1029"/>
         <xdr:cNvCxnSpPr>
@@ -10645,7 +11308,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11610975" y="53359050"/>
-          <a:ext cx="1357313" cy="361950"/>
+          <a:ext cx="1356995" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -10684,7 +11347,7 @@
       <xdr:row>321</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="1031" name="圆角矩形 1030"/>
         <xdr:cNvSpPr/>
@@ -10723,6 +11386,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>编码</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -10741,7 +11405,7 @@
       <xdr:row>321</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="192" name="圆角矩形 191"/>
         <xdr:cNvSpPr/>
@@ -10778,6 +11442,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>解码</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -10786,30 +11451,30 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>638176</xdr:colOff>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>321</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>495301</xdr:colOff>
-      <xdr:row>322</xdr:row>
-      <xdr:rowOff>90489</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
+      <xdr:colOff>475615</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="1036" name="曲线连接符 1035"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="150" idx="1"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8867776" y="55178326"/>
-          <a:ext cx="2600325" cy="119063"/>
+          <a:off x="8772525" y="55168800"/>
+          <a:ext cx="2675890" cy="12700"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 49976"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -10845,7 +11510,7 @@
       <xdr:row>326</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="197" name="圆角矩形 196"/>
         <xdr:cNvSpPr/>
@@ -10882,6 +11547,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>编码</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -10900,7 +11566,7 @@
       <xdr:row>326</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="198" name="圆角矩形 197"/>
         <xdr:cNvSpPr/>
@@ -10939,6 +11605,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>解码</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -11228,53 +11895,57 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A206" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" topLeftCell="A206" workbookViewId="0">
       <selection activeCell="Q222" sqref="Q222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H307" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J321" sqref="J321"/>
+    <sheetView tabSelected="1" topLeftCell="I298" workbookViewId="0">
+      <selection activeCell="V310" sqref="V310"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>